<commit_message>
Updates on Apply Tags and New Inherit Tag from RG
</commit_message>
<xml_diff>
--- a/Scripts/Policies/Tags/Tags-RGs.xlsx
+++ b/Scripts/Policies/Tags/Tags-RGs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Azure\Scripts\Policies\Tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE4E173-13D3-4AD4-BBDD-84B2CBCD04D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66A39D1-3875-435A-A6C6-21A63032AB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>TagName</t>
   </si>
@@ -53,30 +53,12 @@
     <t>ResourceGroupName</t>
   </si>
   <si>
-    <t>cloud-shell-storage-eastus</t>
-  </si>
-  <si>
-    <t>Default-ActivityLogAlerts</t>
-  </si>
-  <si>
-    <t>DefaultResourceGroup-EUS</t>
-  </si>
-  <si>
-    <t>NetworkWatcherRG</t>
-  </si>
-  <si>
-    <t>rg-aspentech-eastus</t>
-  </si>
-  <si>
     <t>rg-FinOps</t>
   </si>
   <si>
     <t>rg-HPC</t>
   </si>
   <si>
-    <t>rg-hub-spoke-lab-eastus</t>
-  </si>
-  <si>
     <t>rg-test1</t>
   </si>
   <si>
@@ -90,24 +72,6 @@
   </si>
   <si>
     <t>Value03</t>
-  </si>
-  <si>
-    <t>Value04</t>
-  </si>
-  <si>
-    <t>Value05</t>
-  </si>
-  <si>
-    <t>Value06</t>
-  </si>
-  <si>
-    <t>Value07</t>
-  </si>
-  <si>
-    <t>Value08</t>
-  </si>
-  <si>
-    <t>Value09</t>
   </si>
 </sst>
 </file>
@@ -431,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,10 +429,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -479,10 +443,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -493,94 +457,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Including Set-Context to handle multiple subscriptions
</commit_message>
<xml_diff>
--- a/Scripts/Policies/Tags/Tags-RGs.xlsx
+++ b/Scripts/Policies/Tags/Tags-RGs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Azure\Scripts\Policies\Tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66A39D1-3875-435A-A6C6-21A63032AB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F34C3-898B-4305-A6D7-FAF753549748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>TagName</t>
   </si>
@@ -47,21 +47,9 @@
     <t>SubscriptionName</t>
   </si>
   <si>
-    <t>MCAPS-MarcusGaspar</t>
-  </si>
-  <si>
     <t>ResourceGroupName</t>
   </si>
   <si>
-    <t>rg-FinOps</t>
-  </si>
-  <si>
-    <t>rg-HPC</t>
-  </si>
-  <si>
-    <t>rg-test1</t>
-  </si>
-  <si>
     <t>FinOps3</t>
   </si>
   <si>
@@ -71,7 +59,16 @@
     <t>Value02</t>
   </si>
   <si>
-    <t>Value03</t>
+    <t>Default - Microsoft Azure Sponsorship 2</t>
+  </si>
+  <si>
+    <t>rg-hpc</t>
+  </si>
+  <si>
+    <t>HPC subscription</t>
+  </si>
+  <si>
+    <t>rg-hpc-eastus</t>
   </si>
 </sst>
 </file>
@@ -395,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -412,7 +409,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -423,44 +420,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New script to Apply Tags to RG (without policies)
</commit_message>
<xml_diff>
--- a/Scripts/Policies/Tags/Tags-RGs.xlsx
+++ b/Scripts/Policies/Tags/Tags-RGs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Azure\Scripts\Policies\Tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F34C3-898B-4305-A6D7-FAF753549748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DBDD5F-9389-4BBE-A7DB-90898112B647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>TagName</t>
   </si>
@@ -53,22 +53,28 @@
     <t>FinOps3</t>
   </si>
   <si>
-    <t>Value01</t>
-  </si>
-  <si>
-    <t>Value02</t>
-  </si>
-  <si>
     <t>Default - Microsoft Azure Sponsorship 2</t>
   </si>
   <si>
-    <t>rg-hpc</t>
-  </si>
-  <si>
     <t>HPC subscription</t>
   </si>
   <si>
-    <t>rg-hpc-eastus</t>
+    <t>SouthCentralUS</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>EastUS</t>
+  </si>
+  <si>
+    <t>rg-hpc-azhop-deploy</t>
+  </si>
+  <si>
+    <t>rg-dev-mg1311-jumpbox</t>
+  </si>
+  <si>
+    <t>Value07</t>
   </si>
 </sst>
 </file>
@@ -392,19 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -417,33 +424,42 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Including some error validations
</commit_message>
<xml_diff>
--- a/Scripts/Policies/Tags/Tags-RGs.xlsx
+++ b/Scripts/Policies/Tags/Tags-RGs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_repo\Azure\Scripts\Policies\Tags\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DBDD5F-9389-4BBE-A7DB-90898112B647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC815CAA-1E25-4D26-8E1F-6F4CA71B91D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>TagName</t>
   </si>
@@ -53,9 +53,6 @@
     <t>FinOps3</t>
   </si>
   <si>
-    <t>Default - Microsoft Azure Sponsorship 2</t>
-  </si>
-  <si>
     <t>HPC subscription</t>
   </si>
   <si>
@@ -74,7 +71,13 @@
     <t>rg-dev-mg1311-jumpbox</t>
   </si>
   <si>
-    <t>Value07</t>
+    <t>Value08</t>
+  </si>
+  <si>
+    <t>Value09</t>
+  </si>
+  <si>
+    <t>Default - Microsoft Azure Sponsorship 3</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,32 +428,32 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -459,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>